<commit_message>
- Menos algoritmos erroneos
</commit_message>
<xml_diff>
--- a/doc/Algoritmos erroneos.xlsx
+++ b/doc/Algoritmos erroneos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Comentario" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Decision_Trees</t>
   </si>
@@ -161,12 +161,6 @@
     <t>Event Covering</t>
   </si>
   <si>
-    <t>Clas-SLIQ</t>
-  </si>
-  <si>
-    <t>Decision Trees</t>
-  </si>
-  <si>
     <t>Genetic Rule Learning</t>
   </si>
   <si>
@@ -176,12 +170,6 @@
     <t>Clas-CORE</t>
   </si>
   <si>
-    <t>Clas-DMEL</t>
-  </si>
-  <si>
-    <t>Clas-GIL</t>
-  </si>
-  <si>
     <t>Clas-ILGA</t>
   </si>
   <si>
@@ -192,12 +180,6 @@
   </si>
   <si>
     <t>Clas-ART</t>
-  </si>
-  <si>
-    <t>Clas-DataSqueezer</t>
-  </si>
-  <si>
-    <t>Clas-Swap1</t>
   </si>
   <si>
     <t>DT-GA</t>
@@ -573,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
@@ -598,17 +580,17 @@
     </row>
     <row r="4" spans="1:5">
       <c r="B4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>27</v>
@@ -634,7 +616,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -687,7 +669,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -717,18 +699,18 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -758,7 +740,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="B37" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -829,27 +811,27 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="B51" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="16.5" customHeight="1">
       <c r="B52" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="16.5" customHeight="1">
       <c r="B53" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="B54" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -902,77 +884,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B17"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
+      <c r="B5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="B8" t="s">
+      <c r="A8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>